<commit_message>
added predictors to socioeconomic model
</commit_message>
<xml_diff>
--- a/analysis/automated/logit_socioeconomic.xlsx
+++ b/analysis/automated/logit_socioeconomic.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,7 +499,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>made_safer ~ age + income + education + homeownership</t>
+          <t>made_safer ~ age + income + sex + education + homeownership + rentmortgage</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -508,20 +508,20 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-0.9409999999999999</v>
+        <v>-1.362</v>
       </c>
       <c r="D2" t="n">
-        <v>0.013</v>
+        <v>0.004</v>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
-        <v>0.018</v>
+        <v>0.024</v>
       </c>
       <c r="G2" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.089</v>
       </c>
       <c r="H2" t="n">
-        <v>473.768</v>
+        <v>483.248</v>
       </c>
     </row>
     <row r="3">
@@ -532,22 +532,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-0.007</v>
+        <v>-0.005</v>
       </c>
       <c r="D3" t="n">
-        <v>0.231</v>
+        <v>0.394</v>
       </c>
       <c r="E3" t="n">
         <v>-0.001</v>
       </c>
       <c r="F3" t="n">
-        <v>0.018</v>
+        <v>0.024</v>
       </c>
       <c r="G3" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.089</v>
       </c>
       <c r="H3" t="n">
-        <v>473.768</v>
+        <v>483.248</v>
       </c>
     </row>
     <row r="4">
@@ -558,22 +558,22 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>-0.061</v>
+        <v>-0.073</v>
       </c>
       <c r="D4" t="n">
-        <v>0.509</v>
+        <v>0.435</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.008999999999999999</v>
+        <v>-0.011</v>
       </c>
       <c r="F4" t="n">
-        <v>0.018</v>
+        <v>0.024</v>
       </c>
       <c r="G4" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.089</v>
       </c>
       <c r="H4" t="n">
-        <v>473.768</v>
+        <v>483.248</v>
       </c>
     </row>
     <row r="5">
@@ -584,22 +584,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.571</v>
+        <v>0.678</v>
       </c>
       <c r="D5" t="n">
-        <v>0.035</v>
+        <v>0.015</v>
       </c>
       <c r="E5" t="n">
-        <v>0.08400000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.018</v>
+        <v>0.024</v>
       </c>
       <c r="G5" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.089</v>
       </c>
       <c r="H5" t="n">
-        <v>473.768</v>
+        <v>483.248</v>
       </c>
     </row>
     <row r="6">
@@ -613,817 +613,813 @@
         <v>-0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.081</v>
+        <v>0.05</v>
       </c>
       <c r="E6" t="n">
         <v>-0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.018</v>
+        <v>0.024</v>
       </c>
       <c r="G6" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.089</v>
       </c>
       <c r="H6" t="n">
-        <v>473.768</v>
+        <v>483.248</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>documents ~ age + income + education + homeownership</t>
-        </is>
-      </c>
+      <c r="A7" s="1" t="n"/>
       <c r="B7" s="1" t="inlineStr">
         <is>
-          <t>Intercept</t>
+          <t>rentmortgage</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>-1.948</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+        <v>0.1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
       <c r="F7" t="n">
-        <v>0.003</v>
+        <v>0.024</v>
       </c>
       <c r="G7" t="n">
-        <v>0.87</v>
+        <v>0.089</v>
       </c>
       <c r="H7" t="n">
-        <v>468.53</v>
+        <v>483.248</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.006</v>
+        <v>0.121</v>
       </c>
       <c r="D8" t="n">
-        <v>0.346</v>
+        <v>0.627</v>
       </c>
       <c r="E8" t="n">
-        <v>0.001</v>
+        <v>0.018</v>
       </c>
       <c r="F8" t="n">
-        <v>0.003</v>
+        <v>0.024</v>
       </c>
       <c r="G8" t="n">
-        <v>0.87</v>
+        <v>0.089</v>
       </c>
       <c r="H8" t="n">
-        <v>468.53</v>
+        <v>483.248</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n"/>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>documents ~ age + income + sex + education + homeownership + rentmortgage</t>
+        </is>
+      </c>
       <c r="B9" s="1" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>Intercept</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.023</v>
+        <v>-2.214</v>
       </c>
       <c r="D9" t="n">
-        <v>0.803</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.003</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
       <c r="G9" t="n">
-        <v>0.87</v>
+        <v>0.907</v>
       </c>
       <c r="H9" t="n">
-        <v>468.53</v>
+        <v>479.964</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
       <c r="B10" s="1" t="inlineStr">
         <is>
-          <t>homeownership</t>
+          <t>age</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.04</v>
+        <v>0.007</v>
       </c>
       <c r="D10" t="n">
-        <v>0.881</v>
+        <v>0.292</v>
       </c>
       <c r="E10" t="n">
-        <v>0.006</v>
+        <v>0.001</v>
       </c>
       <c r="F10" t="n">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
       <c r="G10" t="n">
-        <v>0.87</v>
+        <v>0.907</v>
       </c>
       <c r="H10" t="n">
-        <v>468.53</v>
+        <v>479.964</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n"/>
       <c r="B11" s="1" t="inlineStr">
         <is>
-          <t>income</t>
+          <t>education</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>0.023</v>
       </c>
       <c r="D11" t="n">
-        <v>0.957</v>
+        <v>0.804</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>0.003</v>
       </c>
       <c r="F11" t="n">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
       <c r="G11" t="n">
-        <v>0.87</v>
+        <v>0.907</v>
       </c>
       <c r="H11" t="n">
-        <v>468.53</v>
+        <v>479.964</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>insured ~ age + income + education + homeownership</t>
-        </is>
-      </c>
+      <c r="A12" s="1" t="n"/>
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>Intercept</t>
+          <t>homeownership</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>-1.116</v>
+        <v>0.094</v>
       </c>
       <c r="D12" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="E12" t="inlineStr"/>
+        <v>0.736</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.014</v>
+      </c>
       <c r="F12" t="n">
-        <v>0.029</v>
+        <v>0.005</v>
       </c>
       <c r="G12" t="n">
-        <v>0.007</v>
+        <v>0.907</v>
       </c>
       <c r="H12" t="n">
-        <v>506.883</v>
+        <v>479.964</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n"/>
       <c r="B13" s="1" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>income</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>-0.015</v>
+        <v>-0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.011</v>
+        <v>0.988</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.002</v>
+        <v>-0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.029</v>
+        <v>0.005</v>
       </c>
       <c r="G13" t="n">
-        <v>0.007</v>
+        <v>0.907</v>
       </c>
       <c r="H13" t="n">
-        <v>506.883</v>
+        <v>479.964</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n"/>
       <c r="B14" s="1" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>rentmortgage</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.109</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.209</v>
+        <v>0.464</v>
       </c>
       <c r="E14" t="n">
-        <v>0.018</v>
+        <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.029</v>
+        <v>0.005</v>
       </c>
       <c r="G14" t="n">
-        <v>0.007</v>
+        <v>0.907</v>
       </c>
       <c r="H14" t="n">
-        <v>506.883</v>
+        <v>479.964</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
       <c r="B15" s="1" t="inlineStr">
         <is>
-          <t>homeownership</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.728</v>
+        <v>0.161</v>
       </c>
       <c r="D15" t="n">
+        <v>0.521</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="F15" t="n">
         <v>0.005</v>
       </c>
-      <c r="E15" t="n">
-        <v>0.119</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0.029</v>
-      </c>
       <c r="G15" t="n">
-        <v>0.007</v>
+        <v>0.907</v>
       </c>
       <c r="H15" t="n">
-        <v>506.883</v>
+        <v>479.964</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n"/>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>insured ~ age + income + sex + education + homeownership + rentmortgage</t>
+        </is>
+      </c>
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>income</t>
+          <t>Intercept</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>-0</v>
+        <v>-1.636</v>
       </c>
       <c r="D16" t="n">
-        <v>0.439</v>
-      </c>
-      <c r="E16" t="n">
-        <v>-0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>0.029</v>
+        <v>0.036</v>
       </c>
       <c r="G16" t="n">
         <v>0.007</v>
       </c>
       <c r="H16" t="n">
-        <v>506.883</v>
+        <v>515.598</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>learned_routes ~ age + income + education + homeownership</t>
-        </is>
-      </c>
+      <c r="A17" s="1" t="n"/>
       <c r="B17" s="1" t="inlineStr">
         <is>
-          <t>Intercept</t>
+          <t>age</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>-1.176</v>
+        <v>-0.014</v>
       </c>
       <c r="D17" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="E17" t="inlineStr"/>
+        <v>0.027</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.002</v>
+      </c>
       <c r="F17" t="n">
-        <v>0.001</v>
+        <v>0.036</v>
       </c>
       <c r="G17" t="n">
-        <v>0.985</v>
+        <v>0.007</v>
       </c>
       <c r="H17" t="n">
-        <v>535.692</v>
+        <v>515.598</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n"/>
       <c r="B18" s="1" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>education</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>0.111</v>
       </c>
       <c r="D18" t="n">
-        <v>0.953</v>
+        <v>0.213</v>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>0.018</v>
       </c>
       <c r="F18" t="n">
-        <v>0.001</v>
+        <v>0.036</v>
       </c>
       <c r="G18" t="n">
-        <v>0.985</v>
+        <v>0.007</v>
       </c>
       <c r="H18" t="n">
-        <v>535.692</v>
+        <v>515.598</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n"/>
       <c r="B19" s="1" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>homeownership</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>-0.015</v>
+        <v>0.83</v>
       </c>
       <c r="D19" t="n">
-        <v>0.857</v>
+        <v>0.002</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.003</v>
+        <v>0.134</v>
       </c>
       <c r="F19" t="n">
-        <v>0.001</v>
+        <v>0.036</v>
       </c>
       <c r="G19" t="n">
-        <v>0.985</v>
+        <v>0.007</v>
       </c>
       <c r="H19" t="n">
-        <v>535.692</v>
+        <v>515.598</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n"/>
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>homeownership</t>
+          <t>income</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-0.137</v>
+        <v>-0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.574</v>
+        <v>0.366</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.024</v>
+        <v>-0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.001</v>
+        <v>0.036</v>
       </c>
       <c r="G20" t="n">
-        <v>0.985</v>
+        <v>0.007</v>
       </c>
       <c r="H20" t="n">
-        <v>535.692</v>
+        <v>515.598</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n"/>
       <c r="B21" s="1" t="inlineStr">
         <is>
-          <t>income</t>
+          <t>rentmortgage</t>
         </is>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0.775</v>
+        <v>0.121</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.001</v>
+        <v>0.036</v>
       </c>
       <c r="G21" t="n">
-        <v>0.985</v>
+        <v>0.007</v>
       </c>
       <c r="H21" t="n">
-        <v>535.692</v>
+        <v>515.598</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>supplies ~ age + income + education + homeownership</t>
-        </is>
-      </c>
+      <c r="A22" s="1" t="n"/>
       <c r="B22" s="1" t="inlineStr">
         <is>
+          <t>sex</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0.292</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.223</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.047</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="H22" t="n">
+        <v>515.598</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>learned_routes ~ age + income + sex + education + homeownership + rentmortgage</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
           <t>Intercept</t>
         </is>
       </c>
-      <c r="C22" t="n">
-        <v>-0.211</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.548</v>
-      </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="n">
-        <v>0.026</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="H22" t="n">
-        <v>515.8390000000001</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n"/>
-      <c r="B23" s="1" t="inlineStr">
-        <is>
-          <t>age</t>
-        </is>
-      </c>
       <c r="C23" t="n">
-        <v>-0.018</v>
+        <v>-1.562</v>
       </c>
       <c r="D23" t="n">
-        <v>0.003</v>
-      </c>
-      <c r="E23" t="n">
-        <v>-0.003</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>0.026</v>
+        <v>0.005</v>
       </c>
       <c r="G23" t="n">
-        <v>0.013</v>
+        <v>0.856</v>
       </c>
       <c r="H23" t="n">
-        <v>515.8390000000001</v>
+        <v>545.769</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>age</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>-0.066</v>
+        <v>0.001</v>
       </c>
       <c r="D24" t="n">
-        <v>0.444</v>
+        <v>0.8090000000000001</v>
       </c>
       <c r="E24" t="n">
-        <v>-0.011</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.026</v>
+        <v>0.005</v>
       </c>
       <c r="G24" t="n">
-        <v>0.013</v>
+        <v>0.856</v>
       </c>
       <c r="H24" t="n">
-        <v>515.8390000000001</v>
+        <v>545.769</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n"/>
       <c r="B25" s="1" t="inlineStr">
         <is>
-          <t>homeownership</t>
+          <t>education</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.383</v>
+        <v>-0.013</v>
       </c>
       <c r="D25" t="n">
-        <v>0.129</v>
+        <v>0.881</v>
       </c>
       <c r="E25" t="n">
-        <v>0.064</v>
+        <v>-0.002</v>
       </c>
       <c r="F25" t="n">
-        <v>0.026</v>
+        <v>0.005</v>
       </c>
       <c r="G25" t="n">
-        <v>0.013</v>
+        <v>0.856</v>
       </c>
       <c r="H25" t="n">
-        <v>515.8390000000001</v>
+        <v>545.769</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n"/>
       <c r="B26" s="1" t="inlineStr">
         <is>
+          <t>homeownership</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>-0.066</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.792</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-0.012</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.856</v>
+      </c>
+      <c r="H26" t="n">
+        <v>545.769</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n"/>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
           <t>income</t>
         </is>
       </c>
-      <c r="C26" t="n">
-        <v>-0</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0.281</v>
-      </c>
-      <c r="E26" t="n">
-        <v>-0</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.026</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="H26" t="n">
-        <v>515.8390000000001</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>involved ~ age + income + education + homeownership</t>
-        </is>
-      </c>
-      <c r="B27" s="1" t="inlineStr">
-        <is>
-          <t>Intercept</t>
-        </is>
-      </c>
       <c r="C27" t="n">
-        <v>-0.904</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0.077</v>
-      </c>
-      <c r="E27" t="inlineStr"/>
+        <v>0.844</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
       <c r="F27" t="n">
-        <v>0.08</v>
+        <v>0.005</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>0.856</v>
       </c>
       <c r="H27" t="n">
-        <v>291.354</v>
+        <v>545.769</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n"/>
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>rentmortgage</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>-0.037</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>0.288</v>
       </c>
       <c r="E28" t="n">
-        <v>-0.003</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.08</v>
+        <v>0.005</v>
       </c>
       <c r="G28" t="n">
-        <v>0</v>
+        <v>0.856</v>
       </c>
       <c r="H28" t="n">
-        <v>291.354</v>
+        <v>545.769</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n"/>
       <c r="B29" s="1" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.176</v>
+        <v>0.257</v>
       </c>
       <c r="D29" t="n">
-        <v>0.153</v>
+        <v>0.26</v>
       </c>
       <c r="E29" t="n">
-        <v>0.014</v>
+        <v>0.045</v>
       </c>
       <c r="F29" t="n">
-        <v>0.08</v>
+        <v>0.005</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>0.856</v>
       </c>
       <c r="H29" t="n">
-        <v>291.354</v>
+        <v>545.769</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n"/>
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>supplies ~ age + income + sex + education + homeownership + rentmortgage</t>
+        </is>
+      </c>
       <c r="B30" s="1" t="inlineStr">
         <is>
-          <t>homeownership</t>
+          <t>Intercept</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>-0.742</v>
+        <v>-0.648</v>
       </c>
       <c r="D30" t="n">
-        <v>0.049</v>
-      </c>
-      <c r="E30" t="n">
-        <v>-0.057</v>
-      </c>
+        <v>0.142</v>
+      </c>
+      <c r="E30" t="inlineStr"/>
       <c r="F30" t="n">
-        <v>0.08</v>
+        <v>0.032</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="H30" t="n">
-        <v>291.354</v>
+        <v>524.771</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n"/>
       <c r="B31" s="1" t="inlineStr">
         <is>
-          <t>income</t>
+          <t>age</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>-0.016</v>
       </c>
       <c r="D31" t="n">
-        <v>0.529</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>-0.003</v>
       </c>
       <c r="F31" t="n">
-        <v>0.08</v>
+        <v>0.032</v>
       </c>
       <c r="G31" t="n">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="H31" t="n">
-        <v>291.354</v>
+        <v>524.771</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>made_plan ~ age + income + education + homeownership</t>
-        </is>
-      </c>
+      <c r="A32" s="1" t="n"/>
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>Intercept</t>
+          <t>education</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>-0.624</v>
+        <v>-0.078</v>
       </c>
       <c r="D32" t="n">
-        <v>0.073</v>
-      </c>
-      <c r="E32" t="inlineStr"/>
+        <v>0.374</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-0.013</v>
+      </c>
       <c r="F32" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.032</v>
       </c>
       <c r="G32" t="n">
-        <v>0.335</v>
+        <v>0.013</v>
       </c>
       <c r="H32" t="n">
-        <v>521.491</v>
+        <v>524.771</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n"/>
       <c r="B33" s="1" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>homeownership</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>-0.011</v>
+        <v>0.49</v>
       </c>
       <c r="D33" t="n">
-        <v>0.074</v>
+        <v>0.058</v>
       </c>
       <c r="E33" t="n">
-        <v>-0.002</v>
+        <v>0.081</v>
       </c>
       <c r="F33" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.032</v>
       </c>
       <c r="G33" t="n">
-        <v>0.335</v>
+        <v>0.013</v>
       </c>
       <c r="H33" t="n">
-        <v>521.491</v>
+        <v>524.771</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
       <c r="B34" s="1" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>income</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>-0.07000000000000001</v>
+        <v>-0</v>
       </c>
       <c r="D34" t="n">
-        <v>0.408</v>
+        <v>0.181</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.012</v>
+        <v>-0</v>
       </c>
       <c r="F34" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.032</v>
       </c>
       <c r="G34" t="n">
-        <v>0.335</v>
+        <v>0.013</v>
       </c>
       <c r="H34" t="n">
-        <v>521.491</v>
+        <v>524.771</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n"/>
       <c r="B35" s="1" t="inlineStr">
         <is>
-          <t>homeownership</t>
+          <t>rentmortgage</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>-0.007</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>0.979</v>
+        <v>0.074</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.001</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.032</v>
       </c>
       <c r="G35" t="n">
-        <v>0.335</v>
+        <v>0.013</v>
       </c>
       <c r="H35" t="n">
-        <v>521.491</v>
+        <v>524.771</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n"/>
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>income</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>0.132</v>
       </c>
       <c r="D36" t="n">
-        <v>0.675</v>
+        <v>0.572</v>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>0.022</v>
       </c>
       <c r="F36" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.032</v>
       </c>
       <c r="G36" t="n">
-        <v>0.335</v>
+        <v>0.013</v>
       </c>
       <c r="H36" t="n">
-        <v>521.491</v>
+        <v>524.771</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>practiced_drills ~ age + income + education + homeownership</t>
+          <t>involved ~ age + income + sex + education + homeownership + rentmortgage</t>
         </is>
       </c>
       <c r="B37" s="1" t="inlineStr">
@@ -1432,20 +1428,20 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>-0.913</v>
+        <v>-0.884</v>
       </c>
       <c r="D37" t="n">
-        <v>0.083</v>
+        <v>0.173</v>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
-        <v>0.058</v>
+        <v>0.081</v>
       </c>
       <c r="G37" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="H37" t="n">
-        <v>279.741</v>
+        <v>303.417</v>
       </c>
     </row>
     <row r="38">
@@ -1456,7 +1452,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>-0.037</v>
+        <v>-0.038</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -1465,13 +1461,13 @@
         <v>-0.003</v>
       </c>
       <c r="F38" t="n">
-        <v>0.058</v>
+        <v>0.081</v>
       </c>
       <c r="G38" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="H38" t="n">
-        <v>279.741</v>
+        <v>303.417</v>
       </c>
     </row>
     <row r="39">
@@ -1482,22 +1478,22 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.107</v>
+        <v>0.187</v>
       </c>
       <c r="D39" t="n">
-        <v>0.411</v>
+        <v>0.136</v>
       </c>
       <c r="E39" t="n">
-        <v>0.008</v>
+        <v>0.014</v>
       </c>
       <c r="F39" t="n">
-        <v>0.058</v>
+        <v>0.081</v>
       </c>
       <c r="G39" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="H39" t="n">
-        <v>279.741</v>
+        <v>303.417</v>
       </c>
     </row>
     <row r="40">
@@ -1508,22 +1504,22 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.197</v>
+        <v>-0.765</v>
       </c>
       <c r="D40" t="n">
-        <v>0.606</v>
+        <v>0.049</v>
       </c>
       <c r="E40" t="n">
-        <v>0.014</v>
+        <v>-0.059</v>
       </c>
       <c r="F40" t="n">
-        <v>0.058</v>
+        <v>0.081</v>
       </c>
       <c r="G40" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="H40" t="n">
-        <v>279.741</v>
+        <v>303.417</v>
       </c>
     </row>
     <row r="41">
@@ -1534,300 +1530,824 @@
         </is>
       </c>
       <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.465</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="H41" t="n">
+        <v>303.417</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n"/>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>rentmortgage</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
         <v>-0</v>
       </c>
-      <c r="D41" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="E41" t="n">
+      <c r="D42" t="n">
+        <v>0.712</v>
+      </c>
+      <c r="E42" t="n">
         <v>-0</v>
       </c>
-      <c r="F41" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="H41" t="n">
-        <v>279.741</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>alerts ~ age + income + education + homeownership</t>
-        </is>
-      </c>
-      <c r="B42" s="1" t="inlineStr">
-        <is>
-          <t>Intercept</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
-        <v>-1.722</v>
-      </c>
-      <c r="D42" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" t="inlineStr"/>
       <c r="F42" t="n">
-        <v>0.002</v>
+        <v>0.081</v>
       </c>
       <c r="G42" t="n">
-        <v>0.897</v>
+        <v>0.001</v>
       </c>
       <c r="H42" t="n">
-        <v>486.717</v>
+        <v>303.417</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n"/>
       <c r="B43" s="1" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>sex</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.003</v>
+        <v>0.112</v>
       </c>
       <c r="D43" t="n">
-        <v>0.5649999999999999</v>
+        <v>0.748</v>
       </c>
       <c r="E43" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.081</v>
+      </c>
+      <c r="G43" t="n">
         <v>0.001</v>
       </c>
-      <c r="F43" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0.897</v>
-      </c>
       <c r="H43" t="n">
-        <v>486.717</v>
+        <v>303.417</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n"/>
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>made_plan ~ age + income + sex + education + homeownership + rentmortgage</t>
+        </is>
+      </c>
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>Intercept</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.034</v>
+        <v>-0.962</v>
       </c>
       <c r="D44" t="n">
-        <v>0.707</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0.005</v>
-      </c>
+        <v>0.028</v>
+      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="n">
-        <v>0.002</v>
+        <v>0.014</v>
       </c>
       <c r="G44" t="n">
-        <v>0.897</v>
+        <v>0.35</v>
       </c>
       <c r="H44" t="n">
-        <v>486.717</v>
+        <v>531.668</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n"/>
       <c r="B45" s="1" t="inlineStr">
         <is>
-          <t>homeownership</t>
+          <t>age</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.145</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="D45" t="n">
-        <v>0.581</v>
+        <v>0.139</v>
       </c>
       <c r="E45" t="n">
-        <v>0.022</v>
+        <v>-0.001</v>
       </c>
       <c r="F45" t="n">
-        <v>0.002</v>
+        <v>0.014</v>
       </c>
       <c r="G45" t="n">
-        <v>0.897</v>
+        <v>0.35</v>
       </c>
       <c r="H45" t="n">
-        <v>486.717</v>
+        <v>531.668</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n"/>
       <c r="B46" s="1" t="inlineStr">
         <is>
-          <t>income</t>
+          <t>education</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>-0</v>
+        <v>-0.081</v>
       </c>
       <c r="D46" t="n">
-        <v>0.604</v>
+        <v>0.35</v>
       </c>
       <c r="E46" t="n">
-        <v>-0</v>
+        <v>-0.014</v>
       </c>
       <c r="F46" t="n">
-        <v>0.002</v>
+        <v>0.014</v>
       </c>
       <c r="G46" t="n">
-        <v>0.897</v>
+        <v>0.35</v>
       </c>
       <c r="H46" t="n">
-        <v>486.717</v>
+        <v>531.668</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="inlineStr">
-        <is>
-          <t>family_communication ~ age + income + education + homeownership</t>
-        </is>
-      </c>
+      <c r="A47" s="1" t="n"/>
       <c r="B47" s="1" t="inlineStr">
         <is>
-          <t>Intercept</t>
+          <t>homeownership</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>-1.531</v>
+        <v>0.08</v>
       </c>
       <c r="D47" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="E47" t="inlineStr"/>
+        <v>0.753</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.013</v>
+      </c>
       <c r="F47" t="n">
-        <v>0.025</v>
+        <v>0.014</v>
       </c>
       <c r="G47" t="n">
-        <v>0.097</v>
+        <v>0.35</v>
       </c>
       <c r="H47" t="n">
-        <v>333.305</v>
+        <v>531.668</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n"/>
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>age</t>
+          <t>income</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>-0.021</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>0.013</v>
+        <v>0.871</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.002</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>0.025</v>
+        <v>0.014</v>
       </c>
       <c r="G48" t="n">
-        <v>0.097</v>
+        <v>0.35</v>
       </c>
       <c r="H48" t="n">
-        <v>333.305</v>
+        <v>531.668</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n"/>
       <c r="B49" s="1" t="inlineStr">
         <is>
-          <t>education</t>
+          <t>rentmortgage</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.158</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>0.174</v>
+        <v>0.151</v>
       </c>
       <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
         <v>0.014</v>
       </c>
-      <c r="F49" t="n">
-        <v>0.025</v>
-      </c>
       <c r="G49" t="n">
-        <v>0.097</v>
+        <v>0.35</v>
       </c>
       <c r="H49" t="n">
-        <v>333.305</v>
+        <v>531.668</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n"/>
       <c r="B50" s="1" t="inlineStr">
         <is>
+          <t>sex</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>0.089</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.701</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="H50" t="n">
+        <v>531.668</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>practiced_drills ~ age + income + sex + education + homeownership + rentmortgage</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>Intercept</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>-1.62</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H51" t="n">
+        <v>286.789</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n"/>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>-0.033</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="E52" t="n">
+        <v>-0.002</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H52" t="n">
+        <v>286.789</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n"/>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>education</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.574</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H53" t="n">
+        <v>286.789</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n"/>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
           <t>homeownership</t>
         </is>
       </c>
-      <c r="C50" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="D50" t="n">
-        <v>0.865</v>
-      </c>
-      <c r="E50" t="n">
+      <c r="C54" t="n">
+        <v>0.363</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.351</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H54" t="n">
+        <v>286.789</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n"/>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>income</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>-0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.259</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-0</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H55" t="n">
+        <v>286.789</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n"/>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>rentmortgage</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H56" t="n">
+        <v>286.789</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n"/>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>sex</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.952</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H57" t="n">
+        <v>286.789</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>alerts ~ age + income + sex + education + homeownership + rentmortgage</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>Intercept</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>-2.344</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.378</v>
+      </c>
+      <c r="H58" t="n">
+        <v>493.696</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n"/>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
         <v>0.005</v>
       </c>
-      <c r="F50" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="G50" t="n">
-        <v>0.097</v>
-      </c>
-      <c r="H50" t="n">
-        <v>333.305</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n"/>
-      <c r="B51" s="1" t="inlineStr">
+      <c r="D59" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.378</v>
+      </c>
+      <c r="H59" t="n">
+        <v>493.696</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n"/>
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>education</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.603</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.378</v>
+      </c>
+      <c r="H60" t="n">
+        <v>493.696</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n"/>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>homeownership</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>0.238</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0.381</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.378</v>
+      </c>
+      <c r="H61" t="n">
+        <v>493.696</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n"/>
+      <c r="B62" s="1" t="inlineStr">
         <is>
           <t>income</t>
         </is>
       </c>
-      <c r="C51" t="n">
+      <c r="C62" t="n">
         <v>-0</v>
       </c>
-      <c r="D51" t="n">
-        <v>0.748</v>
-      </c>
-      <c r="E51" t="n">
+      <c r="D62" t="n">
+        <v>0.602</v>
+      </c>
+      <c r="E62" t="n">
         <v>-0</v>
       </c>
-      <c r="F51" t="n">
-        <v>0.025</v>
-      </c>
-      <c r="G51" t="n">
-        <v>0.097</v>
-      </c>
-      <c r="H51" t="n">
-        <v>333.305</v>
+      <c r="F62" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.378</v>
+      </c>
+      <c r="H62" t="n">
+        <v>493.696</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n"/>
+      <c r="B63" s="1" t="inlineStr">
+        <is>
+          <t>rentmortgage</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.223</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.378</v>
+      </c>
+      <c r="H63" t="n">
+        <v>493.696</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n"/>
+      <c r="B64" s="1" t="inlineStr">
+        <is>
+          <t>sex</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>0.505</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.378</v>
+      </c>
+      <c r="H64" t="n">
+        <v>493.696</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>family_communication ~ age + income + sex + education + homeownership + rentmortgage</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="inlineStr">
+        <is>
+          <t>Intercept</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>-2.431</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="H65" t="n">
+        <v>339.925</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n"/>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>-0.018</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-0.002</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="H66" t="n">
+        <v>339.925</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n"/>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>education</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>0.164</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.173</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="H67" t="n">
+        <v>339.925</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n"/>
+      <c r="B68" s="1" t="inlineStr">
+        <is>
+          <t>homeownership</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>0.228</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.514</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="H68" t="n">
+        <v>339.925</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n"/>
+      <c r="B69" s="1" t="inlineStr">
+        <is>
+          <t>income</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>-0</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-0</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="H69" t="n">
+        <v>339.925</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n"/>
+      <c r="B70" s="1" t="inlineStr">
+        <is>
+          <t>rentmortgage</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.055</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="H70" t="n">
+        <v>339.925</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n"/>
+      <c r="B71" s="1" t="inlineStr">
+        <is>
+          <t>sex</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>0.502</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.126</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="H71" t="n">
+        <v>339.925</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A58:A64"/>
+    <mergeCell ref="A16:A22"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="A51:A57"/>
+    <mergeCell ref="A65:A71"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A30:A36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>